<commit_message>
progress on loading new db
</commit_message>
<xml_diff>
--- a/scripts/database/tables/MasterTable.xlsx
+++ b/scripts/database/tables/MasterTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amarok/src/natur-i-norge/scripts/database/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4E4A94A-8820-284F-A165-EC2E0E0FFD07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94A8F5DA-45B4-0843-8833-BBEF350654A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40" yWindow="740" windowWidth="28800" windowHeight="17540" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MajorTypeGroup" sheetId="1" r:id="rId1"/>
@@ -27,6 +27,7 @@
     <sheet name="StandardSegmentElement" sheetId="12" r:id="rId12"/>
     <sheet name="ElementarySegment" sheetId="13" r:id="rId13"/>
     <sheet name="Detail" sheetId="14" r:id="rId14"/>
+    <sheet name="Language" sheetId="15" r:id="rId15"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">LEC!$A$1:$G$1</definedName>
@@ -37,7 +38,7 @@
     <definedName name="nin_MajorType" localSheetId="1">MajorType!$A$1:$A$93</definedName>
     <definedName name="nin_MajorTypeGroup" localSheetId="0">MajorTypeGroup!$A$1:$A$8</definedName>
     <definedName name="nin_MappingScale_1" localSheetId="7">MappingScale!$A$1:$B$6</definedName>
-    <definedName name="nin_MinorType" localSheetId="2">MinorType!$B$1:$C$21</definedName>
+    <definedName name="nin_MinorType" localSheetId="2">MinorType!$B$1:$D$21</definedName>
     <definedName name="nin_MinorTypeScaled" localSheetId="9">MinorTypeScale!$A$1:$C$101</definedName>
     <definedName name="nin_MinorTypeStandardSegment" localSheetId="8">MinorTypeStandardSegment!$A$1:$B$64</definedName>
     <definedName name="nin_PatternOfVariation" localSheetId="3">PatternOfVariation!$A$1:$A$7</definedName>
@@ -60,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4794" uniqueCount="2326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4821" uniqueCount="2348">
   <si>
     <t>_id</t>
   </si>
@@ -7038,6 +7039,72 @@
   </si>
   <si>
     <t>&lt; 10 m2 og største dybde &lt; 1 m</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>Norsk</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>20</t>
   </si>
 </sst>
 </file>
@@ -7405,7 +7472,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -19056,9 +19123,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:E163"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="A2:XFD3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <cols>
+    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="B1" s="4" t="s">
@@ -21830,6 +21902,45 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85C93F20-EC2F-EE4C-8B5B-6369910747A0}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>2192</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2326</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>2195</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2327</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -21837,9 +21948,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G93"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16"/>
   <cols>
@@ -24087,87 +24196,93 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16"/>
   <cols>
-    <col min="2" max="2" width="5.83203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" style="1" customWidth="1"/>
+    <col min="2" max="3" width="5.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16" customHeight="1">
+    <row r="1" spans="1:12" ht="16" customHeight="1">
       <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>1073</v>
+      </c>
+      <c r="D1" t="s">
         <v>410</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>411</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>412</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>413</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>3</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>414</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>415</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="16" customHeight="1">
+    <row r="2" spans="1:12" ht="16" customHeight="1">
       <c r="A2" t="str">
-        <f t="shared" ref="A2:A21" si="0">RIGHT(B2,LEN(B2)-LEN(C2)-1)</f>
+        <f t="shared" ref="A2:A21" si="0">RIGHT(B2,LEN(B2)-LEN(D2)-1)</f>
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>417</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
+        <v>2328</v>
+      </c>
+      <c r="D2" t="s">
         <v>418</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>419</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>420</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>421</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>422</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>423</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>424</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>425</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="16" customHeight="1">
+    <row r="3" spans="1:12" ht="16" customHeight="1">
       <c r="A3" t="str">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -24175,35 +24290,38 @@
       <c r="B3" t="s">
         <v>427</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
+        <v>2329</v>
+      </c>
+      <c r="D3" t="s">
         <v>418</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>428</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>429</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>430</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>431</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>432</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>433</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>434</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="16" customHeight="1">
+    <row r="4" spans="1:12" ht="16" customHeight="1">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -24211,35 +24329,38 @@
       <c r="B4" t="s">
         <v>436</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
+        <v>2330</v>
+      </c>
+      <c r="D4" t="s">
         <v>418</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>437</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>438</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>439</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>440</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>441</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>442</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>443</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="16" customHeight="1">
+    <row r="5" spans="1:12" ht="16" customHeight="1">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -24247,35 +24368,38 @@
       <c r="B5" t="s">
         <v>445</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
+        <v>2331</v>
+      </c>
+      <c r="D5" t="s">
         <v>418</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>446</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>447</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>448</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>449</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>450</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>451</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>452</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="16" customHeight="1">
+    <row r="6" spans="1:12" ht="16" customHeight="1">
       <c r="A6" t="str">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -24283,35 +24407,38 @@
       <c r="B6" t="s">
         <v>454</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
+        <v>2332</v>
+      </c>
+      <c r="D6" t="s">
         <v>418</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>455</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>456</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>457</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>458</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>459</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>460</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>461</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="16" customHeight="1">
+    <row r="7" spans="1:12" ht="16" customHeight="1">
       <c r="A7" t="str">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -24319,35 +24446,38 @@
       <c r="B7" t="s">
         <v>463</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
+        <v>2333</v>
+      </c>
+      <c r="D7" t="s">
         <v>418</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>464</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>465</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>466</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>467</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>468</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>469</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>470</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="16" customHeight="1">
+    <row r="8" spans="1:12" ht="16" customHeight="1">
       <c r="A8" t="str">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -24355,35 +24485,38 @@
       <c r="B8" t="s">
         <v>472</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
+        <v>2334</v>
+      </c>
+      <c r="D8" t="s">
         <v>418</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>473</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>474</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>475</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>476</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>477</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>478</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>479</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="16" customHeight="1">
+    <row r="9" spans="1:12" ht="16" customHeight="1">
       <c r="A9" t="str">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -24391,35 +24524,38 @@
       <c r="B9" t="s">
         <v>481</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
+        <v>2335</v>
+      </c>
+      <c r="D9" t="s">
         <v>418</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>482</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>483</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>484</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>485</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>486</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>487</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>488</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="16" customHeight="1">
+    <row r="10" spans="1:12" ht="16" customHeight="1">
       <c r="A10" t="str">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -24427,35 +24563,38 @@
       <c r="B10" t="s">
         <v>490</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
+        <v>2336</v>
+      </c>
+      <c r="D10" t="s">
         <v>418</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>491</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>492</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>493</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>494</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>495</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>496</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>497</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="16" customHeight="1">
+    <row r="11" spans="1:12" ht="16" customHeight="1">
       <c r="A11" t="str">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -24463,35 +24602,38 @@
       <c r="B11" t="s">
         <v>499</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
+        <v>2337</v>
+      </c>
+      <c r="D11" t="s">
         <v>418</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>500</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>501</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>502</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>503</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>504</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>505</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>506</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="16" customHeight="1">
+    <row r="12" spans="1:12" ht="16" customHeight="1">
       <c r="A12" t="str">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -24499,35 +24641,38 @@
       <c r="B12" t="s">
         <v>508</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1" t="s">
+        <v>2338</v>
+      </c>
+      <c r="D12" t="s">
         <v>418</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>509</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>510</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>511</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>512</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>513</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>514</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>515</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>516</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="16" customHeight="1">
+    <row r="13" spans="1:12" ht="16" customHeight="1">
       <c r="A13" t="str">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -24535,35 +24680,38 @@
       <c r="B13" t="s">
         <v>517</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1" t="s">
+        <v>2339</v>
+      </c>
+      <c r="D13" t="s">
         <v>418</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>518</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>519</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>520</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>521</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>522</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>523</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>524</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="16" customHeight="1">
+    <row r="14" spans="1:12" ht="16" customHeight="1">
       <c r="A14" t="str">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -24571,35 +24719,38 @@
       <c r="B14" t="s">
         <v>526</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="1" t="s">
+        <v>2340</v>
+      </c>
+      <c r="D14" t="s">
         <v>418</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>527</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>528</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>529</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>530</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>531</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
         <v>532</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
         <v>533</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>534</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="16" customHeight="1">
+    <row r="15" spans="1:12" ht="16" customHeight="1">
       <c r="A15" t="str">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -24607,35 +24758,38 @@
       <c r="B15" t="s">
         <v>535</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="1" t="s">
+        <v>2341</v>
+      </c>
+      <c r="D15" t="s">
         <v>418</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>536</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>537</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>529</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>538</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
         <v>539</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
         <v>532</v>
       </c>
-      <c r="J15" t="s">
+      <c r="K15" t="s">
         <v>540</v>
       </c>
-      <c r="K15" t="s">
+      <c r="L15" t="s">
         <v>541</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="16" customHeight="1">
+    <row r="16" spans="1:12" ht="16" customHeight="1">
       <c r="A16" t="str">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -24643,35 +24797,38 @@
       <c r="B16" t="s">
         <v>542</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="1" t="s">
+        <v>2342</v>
+      </c>
+      <c r="D16" t="s">
         <v>418</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>543</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>544</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>545</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>538</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
         <v>546</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J16" t="s">
         <v>547</v>
       </c>
-      <c r="J16" t="s">
+      <c r="K16" t="s">
         <v>548</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L16" t="s">
         <v>541</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="16" customHeight="1">
+    <row r="17" spans="1:12" ht="16" customHeight="1">
       <c r="A17" t="str">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -24679,35 +24836,38 @@
       <c r="B17" t="s">
         <v>549</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="1" t="s">
+        <v>2343</v>
+      </c>
+      <c r="D17" t="s">
         <v>418</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>550</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>551</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>552</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>553</v>
       </c>
-      <c r="H17" t="s">
+      <c r="I17" t="s">
         <v>554</v>
       </c>
-      <c r="I17" t="s">
+      <c r="J17" t="s">
         <v>555</v>
       </c>
-      <c r="J17" t="s">
+      <c r="K17" t="s">
         <v>556</v>
       </c>
-      <c r="K17" t="s">
+      <c r="L17" t="s">
         <v>557</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="16" customHeight="1">
+    <row r="18" spans="1:12" ht="16" customHeight="1">
       <c r="A18" t="str">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -24715,35 +24875,38 @@
       <c r="B18" t="s">
         <v>558</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="1" t="s">
+        <v>2344</v>
+      </c>
+      <c r="D18" t="s">
         <v>418</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>559</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>560</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>561</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>562</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
         <v>563</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J18" t="s">
         <v>564</v>
       </c>
-      <c r="J18" t="s">
+      <c r="K18" t="s">
         <v>565</v>
       </c>
-      <c r="K18" t="s">
+      <c r="L18" t="s">
         <v>566</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="16" customHeight="1">
+    <row r="19" spans="1:12" ht="16" customHeight="1">
       <c r="A19" t="str">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -24751,35 +24914,38 @@
       <c r="B19" t="s">
         <v>567</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="1" t="s">
+        <v>2345</v>
+      </c>
+      <c r="D19" t="s">
         <v>418</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>568</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>569</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>570</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>571</v>
       </c>
-      <c r="H19" t="s">
+      <c r="I19" t="s">
         <v>572</v>
       </c>
-      <c r="I19" t="s">
+      <c r="J19" t="s">
         <v>573</v>
       </c>
-      <c r="J19" t="s">
+      <c r="K19" t="s">
         <v>574</v>
       </c>
-      <c r="K19" t="s">
+      <c r="L19" t="s">
         <v>575</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="16" customHeight="1">
+    <row r="20" spans="1:12" ht="16" customHeight="1">
       <c r="A20" t="str">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -24787,35 +24953,38 @@
       <c r="B20" t="s">
         <v>576</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="1" t="s">
+        <v>2346</v>
+      </c>
+      <c r="D20" t="s">
         <v>418</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>577</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>578</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>579</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>580</v>
       </c>
-      <c r="H20" t="s">
+      <c r="I20" t="s">
         <v>581</v>
       </c>
-      <c r="I20" t="s">
+      <c r="J20" t="s">
         <v>582</v>
       </c>
-      <c r="J20" t="s">
+      <c r="K20" t="s">
         <v>583</v>
       </c>
-      <c r="K20" t="s">
+      <c r="L20" t="s">
         <v>584</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="16" customHeight="1">
+    <row r="21" spans="1:12" ht="16" customHeight="1">
       <c r="A21" t="str">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -24823,31 +24992,34 @@
       <c r="B21" t="s">
         <v>585</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="1" t="s">
+        <v>2347</v>
+      </c>
+      <c r="D21" t="s">
         <v>418</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>586</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>587</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>588</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>589</v>
       </c>
-      <c r="H21" t="s">
+      <c r="I21" t="s">
         <v>590</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
         <v>591</v>
       </c>
-      <c r="J21" t="s">
+      <c r="K21" t="s">
         <v>592</v>
       </c>
-      <c r="K21" t="s">
+      <c r="L21" t="s">
         <v>593</v>
       </c>
     </row>

</xml_diff>